<commit_message>
Putting it in HFS
</commit_message>
<xml_diff>
--- a/Wknd_Sched_Builder/AssignmentList.xlsx
+++ b/Wknd_Sched_Builder/AssignmentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloned_Repositories\HFS_Gradio_Projects\Wknd_Sched_Builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35106977-F142-4D3C-B2D3-573D62664B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC0344C-D18A-4E2D-85F7-E1E5B79EE0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35565" yWindow="1695" windowWidth="21600" windowHeight="11235" tabRatio="707" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1092" windowWidth="21624" windowHeight="11244" tabRatio="707" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All_Slots" sheetId="4" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="223">
   <si>
     <t>AssnType</t>
   </si>
@@ -517,9 +517,6 @@
     <t>Keg Line</t>
   </si>
   <si>
-    <t>Keg CIP</t>
-  </si>
-  <si>
     <t>Variopak support</t>
   </si>
   <si>
@@ -779,6 +776,42 @@
   </si>
   <si>
     <t>Pouch Packer6</t>
+  </si>
+  <si>
+    <t>Bott Supp Ht Rlf 1</t>
+  </si>
+  <si>
+    <t>Bott Supp Ht Rlf 2</t>
+  </si>
+  <si>
+    <t>Filler Sweep 1</t>
+  </si>
+  <si>
+    <t>Filler Sweep 2</t>
+  </si>
+  <si>
+    <t>Carton Aid 1</t>
+  </si>
+  <si>
+    <t>Carton Aid 2</t>
+  </si>
+  <si>
+    <t>Packer Ht Brk</t>
+  </si>
+  <si>
+    <t>Keg</t>
+  </si>
+  <si>
+    <t>E De Veyra Sat</t>
+  </si>
+  <si>
+    <t>E De Veyra Sun</t>
+  </si>
+  <si>
+    <t>Z Cook Sat</t>
+  </si>
+  <si>
+    <t>Z Cook Sun</t>
   </si>
 </sst>
 </file>
@@ -871,7 +904,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -900,6 +933,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1525,8 +1562,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CE372191-17FC-4397-A620-B28088C8812B}" name="All_Slots" displayName="All_Slots" ref="A1:G31" totalsRowShown="0">
-  <autoFilter ref="A1:G31" xr:uid="{059D1060-D207-4B9D-A006-CF0431D6758F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CE372191-17FC-4397-A620-B28088C8812B}" name="All_Slots" displayName="All_Slots" ref="A1:G38" totalsRowShown="0">
+  <autoFilter ref="A1:G38" xr:uid="{059D1060-D207-4B9D-A006-CF0431D6758F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{2CC27B11-A292-426B-97B6-7130C8C9D4F3}" name="Start Slot"/>
     <tableColumn id="2" xr3:uid="{8A152051-0D61-47D6-BFEC-594E995E4F1D}" name="End Slot"/>
@@ -1545,8 +1582,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F6C12A1D-C9D6-49E0-90A8-78F7AE1B2444}" name="Assn_List" displayName="Assn_List" ref="A1:I86" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:I86" xr:uid="{F6C12A1D-C9D6-49E0-90A8-78F7AE1B2444}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F6C12A1D-C9D6-49E0-90A8-78F7AE1B2444}" name="Assn_List" displayName="Assn_List" ref="A1:I90" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:I90" xr:uid="{F6C12A1D-C9D6-49E0-90A8-78F7AE1B2444}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BF1A4BE0-533F-4D33-902B-4B0793170CE5}" name="Active?" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{BD0C2663-572B-49CB-B47A-8EBC47F49069}" name="AssnType" dataDxfId="10"/>
@@ -1579,8 +1616,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B5394865-9CC8-4FF3-A5B4-D7D7B5491B25}" name="TrainAssnMtx" displayName="TrainAssnMtx" ref="A1:B61" totalsRowShown="0" dataDxfId="2">
-  <autoFilter ref="A1:B61" xr:uid="{B5394865-9CC8-4FF3-A5B4-D7D7B5491B25}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B5394865-9CC8-4FF3-A5B4-D7D7B5491B25}" name="TrainAssnMtx" displayName="TrainAssnMtx" ref="A1:B68" totalsRowShown="0" dataDxfId="2">
+  <autoFilter ref="A1:B68" xr:uid="{B5394865-9CC8-4FF3-A5B4-D7D7B5491B25}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A5250A11-FD2F-47C9-ABD9-9A441218134C}" name="Display_Name" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{F2284C7C-D714-44C5-A91E-0A5ADCBD9330}" name="Train_Mtx_Name" dataDxfId="0"/>
@@ -1852,10 +1889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96EE401-FD5B-4675-8E2B-71951E8EAC3D}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1892,177 +1929,184 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="9" t="str">
+        <v>211</v>
+      </c>
+      <c r="D2" s="14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Sat / 3a-7a</v>
-      </c>
-      <c r="E2" s="9" t="str">
+        <v>Sat / 11a-3p</v>
+      </c>
+      <c r="E2" s="14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Sun / 3a-7a</v>
+        <v>Sat / 7p-11p</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="str">
+        <v>212</v>
+      </c>
+      <c r="D3" s="14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Fri / 11p(Thurs)-3a(Fri)</v>
-      </c>
-      <c r="E3" t="str">
+        <v>Sat / 11a-3p</v>
+      </c>
+      <c r="E3" s="14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Mon / 7p-11p</v>
-      </c>
+        <v>Sat / 7p-11p</v>
+      </c>
+      <c r="F3" s="9"/>
       <c r="G3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" t="str">
+        <v>12</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D4" s="14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Fri / 11p(Thurs)-3a(Fri)</v>
-      </c>
-      <c r="E4" t="str">
+        <v>Sat / 11a-3p</v>
+      </c>
+      <c r="E4" s="14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Mon / 7p-11p</v>
-      </c>
+        <v>Sat / 7p-11p</v>
+      </c>
+      <c r="F4" s="9"/>
       <c r="G4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="str">
+        <v>12</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D5" s="14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Fri / 11p(Thurs)-3a(Fri)</v>
-      </c>
-      <c r="E5" t="str">
+        <v>Sat / 11a-3p</v>
+      </c>
+      <c r="E5" s="14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Mon / 7p-11p</v>
-      </c>
+        <v>Sat / 7p-11p</v>
+      </c>
+      <c r="F5" s="9"/>
       <c r="G5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B6">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" t="str">
+        <v>211</v>
+      </c>
+      <c r="D6" s="14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Fri / 11p(Thurs)-3a(Fri)</v>
-      </c>
-      <c r="E6" t="str">
+        <v>Sun / 11a-3p</v>
+      </c>
+      <c r="E6" s="14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Mon / 7p-11p</v>
-      </c>
+        <v>Mon / 11p(Sun)-3a(Mon)</v>
+      </c>
+      <c r="F6" s="9"/>
       <c r="G6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B7">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D7" t="str">
+        <v>212</v>
+      </c>
+      <c r="D7" s="14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Fri / 11p(Thurs)-3a(Fri)</v>
-      </c>
-      <c r="E7" t="str">
+        <v>Sun / 11a-3p</v>
+      </c>
+      <c r="E7" s="14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Mon / 7p-11p</v>
-      </c>
+        <v>Mon / 11p(Sun)-3a(Mon)</v>
+      </c>
+      <c r="F7" s="9"/>
       <c r="G7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B8">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" t="str">
+        <v>19</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D8" s="14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Fri / 11p(Thurs)-3a(Fri)</v>
-      </c>
-      <c r="E8" t="str">
+        <v>Sun / 11a-3p</v>
+      </c>
+      <c r="E8" s="14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Mon / 7p-11p</v>
-      </c>
+        <v>Mon / 11p(Sun)-3a(Mon)</v>
+      </c>
+      <c r="F8" s="9"/>
       <c r="G8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B9">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" t="str">
+        <v>19</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D9" s="14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Fri / 11p(Thurs)-3a(Fri)</v>
-      </c>
-      <c r="E9" t="str">
+        <v>Sun / 11a-3p</v>
+      </c>
+      <c r="E9" s="14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Mon / 7p-11p</v>
-      </c>
+        <v>Mon / 11p(Sun)-3a(Mon)</v>
+      </c>
+      <c r="F9" s="9"/>
       <c r="G9">
         <v>1</v>
       </c>
@@ -2075,7 +2119,7 @@
         <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="D10" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2097,7 +2141,7 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D11" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2119,7 +2163,7 @@
         <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="D12" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2141,7 +2185,7 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>125</v>
       </c>
       <c r="D13" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2163,7 +2207,7 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
       <c r="D14" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2185,7 +2229,7 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D15" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2207,7 +2251,7 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D16" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2229,7 +2273,7 @@
         <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D17" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2251,7 +2295,7 @@
         <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2273,7 +2317,7 @@
         <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D19" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2294,8 +2338,8 @@
       <c r="B20">
         <v>24</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>106</v>
+      <c r="C20" t="s">
+        <v>83</v>
       </c>
       <c r="D20" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2316,8 +2360,8 @@
       <c r="B21">
         <v>24</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>108</v>
+      <c r="C21" t="s">
+        <v>49</v>
       </c>
       <c r="D21" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2338,8 +2382,8 @@
       <c r="B22">
         <v>24</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>111</v>
+      <c r="C22" t="s">
+        <v>84</v>
       </c>
       <c r="D22" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2360,8 +2404,8 @@
       <c r="B23">
         <v>24</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>128</v>
+      <c r="C23" t="s">
+        <v>81</v>
       </c>
       <c r="D23" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2382,8 +2426,8 @@
       <c r="B24">
         <v>24</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>105</v>
+      <c r="C24" t="s">
+        <v>82</v>
       </c>
       <c r="D24" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2405,7 +2449,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>205</v>
+        <v>78</v>
       </c>
       <c r="D25" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2415,9 +2459,6 @@
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
         <v>Mon / 7p-11p</v>
       </c>
-      <c r="F25" t="s">
-        <v>125</v>
-      </c>
       <c r="G25">
         <v>1</v>
       </c>
@@ -2429,8 +2470,8 @@
       <c r="B26">
         <v>24</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>118</v>
+      <c r="C26" t="s">
+        <v>85</v>
       </c>
       <c r="D26" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2452,7 +2493,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D27" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2474,7 +2515,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="D28" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2496,7 +2537,7 @@
         <v>24</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D29" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2518,7 +2559,7 @@
         <v>24</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="D30" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2534,30 +2575,188 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B31">
-        <v>16</v>
-      </c>
-      <c r="C31" t="s">
-        <v>123</v>
+        <v>24</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>105</v>
       </c>
       <c r="D31" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Sun / 7a-11a</v>
+        <v>Fri / 11p(Thurs)-3a(Fri)</v>
       </c>
       <c r="E31" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Sun / 11a-3p</v>
-      </c>
-      <c r="F31" t="s">
+        <v>Mon / 7p-11p</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>204</v>
+      </c>
+      <c r="D32" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Fri / 11p(Thurs)-3a(Fri)</v>
+      </c>
+      <c r="E32" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Mon / 7p-11p</v>
+      </c>
+      <c r="F32" t="s">
         <v>124</v>
       </c>
-      <c r="G31">
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>24</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Fri / 11p(Thurs)-3a(Fri)</v>
+      </c>
+      <c r="E33" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Mon / 7p-11p</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>24</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Fri / 11p(Thurs)-3a(Fri)</v>
+      </c>
+      <c r="E34" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Mon / 7p-11p</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>24</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Fri / 11p(Thurs)-3a(Fri)</v>
+      </c>
+      <c r="E35" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Mon / 7p-11p</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>24</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Fri / 11p(Thurs)-3a(Fri)</v>
+      </c>
+      <c r="E36" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Mon / 7p-11p</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>24</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Fri / 11p(Thurs)-3a(Fri)</v>
+      </c>
+      <c r="E37" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Mon / 7p-11p</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>13</v>
+      </c>
+      <c r="B38">
+        <v>18</v>
+      </c>
+      <c r="C38" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[Start Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Sun / 11p(Sat)-3a(Sun)</v>
+      </c>
+      <c r="E38" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(All_Slots[[#This Row],[End Slot]],[1]Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Sun / 7p-11p</v>
+      </c>
+      <c r="F38" t="s">
+        <v>218</v>
+      </c>
+      <c r="G38">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -2568,10 +2767,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2621,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C2" s="2">
         <v>7</v>
@@ -2644,7 +2843,7 @@
         <v>Sat / 3a-7a</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2652,7 +2851,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3" s="2">
         <v>9</v>
@@ -2675,7 +2874,7 @@
         <v>Sat / 3p-7p</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -2704,7 +2903,7 @@
         <v>Sun / 3a-7a</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -2840,7 +3039,7 @@
         <v>7104444</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G9" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C9,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C9,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -2871,7 +3070,7 @@
         <v>7401166</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G10" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C10,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C10,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3243,7 +3442,7 @@
         <v>7403058</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G22" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C22,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C22,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3420,27 +3619,27 @@
         <v>4</v>
       </c>
       <c r="C28" s="2">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D28" s="2">
-        <v>15</v>
-      </c>
-      <c r="E28" s="2">
-        <v>7402632</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" s="2" t="str">
+        <v>9</v>
+      </c>
+      <c r="E28" s="7">
+        <v>7104857</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G28" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C28,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C28,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Sun / 11p(Sat)-3a(Sun)</v>
-      </c>
-      <c r="H28" s="2" t="str">
+        <v>Sat / 11p(Fri)-3a(Sat)</v>
+      </c>
+      <c r="H28" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D28,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D28,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Sun / 7a-11a</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>146</v>
+        <v>Sat / 7a-11a</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -3457,10 +3656,10 @@
         <v>15</v>
       </c>
       <c r="E29" s="2">
-        <v>7400336</v>
+        <v>7402632</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="G29" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C29,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C29,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3471,7 +3670,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -3487,11 +3686,11 @@
       <c r="D30" s="2">
         <v>15</v>
       </c>
-      <c r="E30" s="7">
-        <v>7104444</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>126</v>
+      <c r="E30" s="2">
+        <v>7400336</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="G30" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C30,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C30,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3501,8 +3700,8 @@
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D30,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D30,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
         <v>Sun / 7a-11a</v>
       </c>
-      <c r="I30" s="7" t="s">
-        <v>148</v>
+      <c r="I30" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -3519,10 +3718,10 @@
         <v>15</v>
       </c>
       <c r="E31" s="7">
-        <v>7401166</v>
+        <v>7104444</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G31" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C31,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C31,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3533,7 +3732,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -3550,10 +3749,10 @@
         <v>15</v>
       </c>
       <c r="E32" s="7">
-        <v>7096593</v>
+        <v>7401166</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="G32" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C32,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C32,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3564,7 +3763,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -3581,10 +3780,10 @@
         <v>15</v>
       </c>
       <c r="E33" s="7">
-        <v>7095864</v>
+        <v>7096593</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G33" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C33,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C33,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3595,7 +3794,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -3612,10 +3811,10 @@
         <v>15</v>
       </c>
       <c r="E34" s="7">
-        <v>7097996</v>
+        <v>7095864</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G34" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C34,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C34,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3626,7 +3825,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -3643,21 +3842,21 @@
         <v>15</v>
       </c>
       <c r="E35" s="7">
-        <v>7093500</v>
+        <v>7097996</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G35" s="7" t="str">
+        <v>76</v>
+      </c>
+      <c r="G35" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C35,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C35,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
         <v>Sun / 11p(Sat)-3a(Sun)</v>
       </c>
-      <c r="H35" s="7" t="str">
+      <c r="H35" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D35,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D35,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -3674,10 +3873,10 @@
         <v>15</v>
       </c>
       <c r="E36" s="7">
-        <v>7400330</v>
+        <v>7093500</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G36" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C36,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C36,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3688,7 +3887,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -3705,10 +3904,10 @@
         <v>15</v>
       </c>
       <c r="E37" s="7">
-        <v>7096286</v>
+        <v>7400330</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G37" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C37,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C37,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3719,7 +3918,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -3736,10 +3935,10 @@
         <v>15</v>
       </c>
       <c r="E38" s="7">
-        <v>7401878</v>
+        <v>7096286</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G38" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C38,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C38,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3750,7 +3949,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -3767,10 +3966,10 @@
         <v>15</v>
       </c>
       <c r="E39" s="7">
-        <v>7095136</v>
+        <v>7401878</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G39" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C39,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C39,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3781,7 +3980,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -3798,10 +3997,10 @@
         <v>15</v>
       </c>
       <c r="E40" s="7">
-        <v>7094183</v>
+        <v>7095136</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="G40" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C40,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C40,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3812,7 +4011,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -3829,10 +4028,10 @@
         <v>15</v>
       </c>
       <c r="E41" s="7">
-        <v>7077415</v>
+        <v>7094183</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G41" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C41,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C41,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3843,7 +4042,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -3860,10 +4059,10 @@
         <v>15</v>
       </c>
       <c r="E42" s="7">
-        <v>7090966</v>
+        <v>7077415</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G42" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C42,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C42,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3874,7 +4073,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -3890,11 +4089,11 @@
       <c r="D43" s="2">
         <v>15</v>
       </c>
-      <c r="E43" s="13">
-        <v>7403058</v>
+      <c r="E43" s="7">
+        <v>7090966</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="G43" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C43,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C43,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3905,7 +4104,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -3921,11 +4120,11 @@
       <c r="D44" s="2">
         <v>15</v>
       </c>
-      <c r="E44" s="7">
-        <v>7077878</v>
+      <c r="E44" s="13">
+        <v>7403058</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="G44" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C44,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C44,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3936,7 +4135,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -3953,10 +4152,10 @@
         <v>15</v>
       </c>
       <c r="E45" s="7">
-        <v>7099948</v>
+        <v>7077878</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G45" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C45,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C45,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3967,7 +4166,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -3984,10 +4183,10 @@
         <v>15</v>
       </c>
       <c r="E46" s="7">
-        <v>7403656</v>
+        <v>7099948</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G46" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C46,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C46,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -3998,7 +4197,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
@@ -4015,10 +4214,10 @@
         <v>15</v>
       </c>
       <c r="E47" s="7">
-        <v>7104560</v>
+        <v>7403656</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G47" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C47,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C47,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4029,7 +4228,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
@@ -4046,10 +4245,10 @@
         <v>15</v>
       </c>
       <c r="E48" s="7">
-        <v>7403267</v>
+        <v>7104560</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G48" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C48,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C48,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4060,7 +4259,7 @@
         <v>Sun / 7a-11a</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
@@ -4071,27 +4270,27 @@
         <v>4</v>
       </c>
       <c r="C49" s="2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D49" s="2">
-        <v>12</v>
-      </c>
-      <c r="E49" s="2">
-        <v>7403368</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G49" s="2" t="str">
+        <v>15</v>
+      </c>
+      <c r="E49" s="7">
+        <v>7403267</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G49" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C49,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C49,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Sat / 11a-3p</v>
-      </c>
-      <c r="H49" s="2" t="str">
+        <v>Sun / 11p(Sat)-3a(Sun)</v>
+      </c>
+      <c r="H49" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D49,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D49,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Sat / 7p-11p</v>
+        <v>Sun / 7a-11a</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -4102,27 +4301,27 @@
         <v>4</v>
       </c>
       <c r="C50" s="2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D50" s="2">
-        <v>12</v>
-      </c>
-      <c r="E50" s="2">
-        <v>7403455</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G50" s="2" t="str">
+        <v>15</v>
+      </c>
+      <c r="E50" s="7">
+        <v>7104857</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G50" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C50,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C50,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Sat / 11a-3p</v>
-      </c>
-      <c r="H50" s="2" t="str">
+        <v>Sun / 11p(Sat)-3a(Sun)</v>
+      </c>
+      <c r="H50" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D50,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D50,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Sat / 7p-11p</v>
+        <v>Sun / 7a-11a</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>168</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -4138,11 +4337,11 @@
       <c r="D51" s="2">
         <v>12</v>
       </c>
-      <c r="E51" s="7">
-        <v>7104178</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>126</v>
+      <c r="E51" s="2">
+        <v>7403368</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="G51" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C51,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C51,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4153,7 +4352,7 @@
         <v>Sat / 7p-11p</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -4169,11 +4368,11 @@
       <c r="D52" s="2">
         <v>12</v>
       </c>
-      <c r="E52" s="7">
-        <v>7096844</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>127</v>
+      <c r="E52" s="2">
+        <v>7403455</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="G52" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C52,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C52,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4184,7 +4383,7 @@
         <v>Sat / 7p-11p</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -4201,10 +4400,10 @@
         <v>12</v>
       </c>
       <c r="E53" s="7">
-        <v>7401165</v>
+        <v>7104178</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="G53" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C53,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C53,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4215,7 +4414,7 @@
         <v>Sat / 7p-11p</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -4232,10 +4431,10 @@
         <v>12</v>
       </c>
       <c r="E54" s="7">
-        <v>7401949</v>
+        <v>7096844</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>75</v>
+        <v>126</v>
       </c>
       <c r="G54" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C54,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C54,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4246,7 +4445,7 @@
         <v>Sat / 7p-11p</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
@@ -4263,10 +4462,10 @@
         <v>12</v>
       </c>
       <c r="E55" s="7">
-        <v>7401950</v>
+        <v>7401165</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G55" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C55,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C55,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4277,7 +4476,7 @@
         <v>Sat / 7p-11p</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -4294,21 +4493,21 @@
         <v>12</v>
       </c>
       <c r="E56" s="7">
-        <v>7095749</v>
+        <v>7401949</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G56" s="7" t="str">
+        <v>75</v>
+      </c>
+      <c r="G56" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C56,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C56,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
         <v>Sat / 11a-3p</v>
       </c>
-      <c r="H56" s="7" t="str">
+      <c r="H56" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D56,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D56,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
         <v>Sat / 7p-11p</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
@@ -4325,21 +4524,21 @@
         <v>12</v>
       </c>
       <c r="E57" s="7">
-        <v>7091824</v>
-      </c>
-      <c r="F57" t="s">
-        <v>49</v>
-      </c>
-      <c r="G57" s="7" t="str">
+        <v>7401950</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G57" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C57,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C57,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
         <v>Sat / 11a-3p</v>
       </c>
-      <c r="H57" s="7" t="str">
+      <c r="H57" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D57,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D57,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
         <v>Sat / 7p-11p</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
@@ -4356,10 +4555,10 @@
         <v>12</v>
       </c>
       <c r="E58" s="7">
-        <v>7402915</v>
+        <v>7095749</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G58" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C58,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C58,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4370,7 +4569,7 @@
         <v>Sat / 7p-11p</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
@@ -4387,10 +4586,10 @@
         <v>12</v>
       </c>
       <c r="E59" s="7">
-        <v>7051907</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>78</v>
+        <v>7091824</v>
+      </c>
+      <c r="F59" t="s">
+        <v>49</v>
       </c>
       <c r="G59" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C59,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C59,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4401,7 +4600,7 @@
         <v>Sat / 7p-11p</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
@@ -4418,10 +4617,10 @@
         <v>12</v>
       </c>
       <c r="E60" s="7">
-        <v>7400976</v>
+        <v>7402915</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G60" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C60,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C60,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4432,7 +4631,7 @@
         <v>Sat / 7p-11p</v>
       </c>
       <c r="I60" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
@@ -4449,10 +4648,10 @@
         <v>12</v>
       </c>
       <c r="E61" s="7">
-        <v>7400954</v>
+        <v>7051907</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="G61" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C61,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C61,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4463,7 +4662,7 @@
         <v>Sat / 7p-11p</v>
       </c>
       <c r="I61" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
@@ -4480,10 +4679,10 @@
         <v>12</v>
       </c>
       <c r="E62" s="7">
-        <v>7051890</v>
+        <v>7400976</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="G62" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C62,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C62,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4494,7 +4693,7 @@
         <v>Sat / 7p-11p</v>
       </c>
       <c r="I62" s="7" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
@@ -4511,10 +4710,10 @@
         <v>12</v>
       </c>
       <c r="E63" s="7">
-        <v>7051891</v>
+        <v>7400954</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G63" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C63,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C63,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4525,7 +4724,7 @@
         <v>Sat / 7p-11p</v>
       </c>
       <c r="I63" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
@@ -4542,10 +4741,10 @@
         <v>12</v>
       </c>
       <c r="E64" s="7">
-        <v>7403004</v>
+        <v>7051890</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="G64" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C64,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C64,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4556,7 +4755,7 @@
         <v>Sat / 7p-11p</v>
       </c>
       <c r="I64" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -4573,10 +4772,10 @@
         <v>12</v>
       </c>
       <c r="E65" s="7">
-        <v>7095152</v>
+        <v>7051891</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G65" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C65,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C65,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4587,7 +4786,7 @@
         <v>Sat / 7p-11p</v>
       </c>
       <c r="I65" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -4604,10 +4803,10 @@
         <v>12</v>
       </c>
       <c r="E66" s="7">
-        <v>7095156</v>
+        <v>7403004</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="G66" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C66,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C66,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4618,7 +4817,7 @@
         <v>Sat / 7p-11p</v>
       </c>
       <c r="I66" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
@@ -4635,10 +4834,10 @@
         <v>12</v>
       </c>
       <c r="E67" s="7">
-        <v>7051908</v>
+        <v>7095152</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G67" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C67,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C67,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4660,27 +4859,27 @@
         <v>4</v>
       </c>
       <c r="C68" s="2">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D68" s="2">
-        <v>18</v>
-      </c>
-      <c r="E68" s="2">
-        <v>7403368</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G68" s="2" t="str">
+        <v>12</v>
+      </c>
+      <c r="E68" s="7">
+        <v>7095156</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G68" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C68,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C68,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Sun / 11a-3p</v>
-      </c>
-      <c r="H68" s="2" t="str">
+        <v>Sat / 11a-3p</v>
+      </c>
+      <c r="H68" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D68,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D68,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Sun / 7p-11p</v>
+        <v>Sat / 7p-11p</v>
       </c>
       <c r="I68" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
@@ -4691,27 +4890,27 @@
         <v>4</v>
       </c>
       <c r="C69" s="2">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D69" s="2">
-        <v>18</v>
-      </c>
-      <c r="E69" s="2">
-        <v>7403455</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G69" s="2" t="str">
+        <v>12</v>
+      </c>
+      <c r="E69" s="7">
+        <v>7051908</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G69" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C69,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C69,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Sun / 11a-3p</v>
-      </c>
-      <c r="H69" s="2" t="str">
+        <v>Sat / 11a-3p</v>
+      </c>
+      <c r="H69" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D69,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D69,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Sun / 7p-11p</v>
+        <v>Sat / 7p-11p</v>
       </c>
       <c r="I69" s="7" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
@@ -4722,27 +4921,27 @@
         <v>4</v>
       </c>
       <c r="C70" s="2">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D70" s="2">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E70" s="7">
-        <v>7104178</v>
+        <v>7104754</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="G70" s="2" t="str">
+        <v>84</v>
+      </c>
+      <c r="G70" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C70,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C70,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Sun / 11a-3p</v>
-      </c>
-      <c r="H70" s="2" t="str">
+        <v>Sat / 11a-3p</v>
+      </c>
+      <c r="H70" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D70,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D70,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
-        <v>Sun / 7p-11p</v>
+        <v>Sat / 7p-11p</v>
       </c>
       <c r="I70" s="7" t="s">
-        <v>188</v>
+        <v>221</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
@@ -4758,11 +4957,11 @@
       <c r="D71" s="2">
         <v>18</v>
       </c>
-      <c r="E71" s="7">
-        <v>7096844</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>127</v>
+      <c r="E71" s="2">
+        <v>7403368</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="G71" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C71,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C71,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4773,7 +4972,7 @@
         <v>Sun / 7p-11p</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
@@ -4789,11 +4988,11 @@
       <c r="D72" s="2">
         <v>18</v>
       </c>
-      <c r="E72" s="7">
-        <v>7401165</v>
-      </c>
-      <c r="F72" s="7" t="s">
-        <v>74</v>
+      <c r="E72" s="2">
+        <v>7403455</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="G72" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C72,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C72,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4804,7 +5003,7 @@
         <v>Sun / 7p-11p</v>
       </c>
       <c r="I72" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
@@ -4821,10 +5020,10 @@
         <v>18</v>
       </c>
       <c r="E73" s="7">
-        <v>7401949</v>
+        <v>7104178</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="G73" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C73,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C73,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4835,7 +5034,7 @@
         <v>Sun / 7p-11p</v>
       </c>
       <c r="I73" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
@@ -4852,10 +5051,10 @@
         <v>18</v>
       </c>
       <c r="E74" s="7">
-        <v>7401950</v>
+        <v>7096844</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>76</v>
+        <v>126</v>
       </c>
       <c r="G74" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C74,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C74,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4866,7 +5065,7 @@
         <v>Sun / 7p-11p</v>
       </c>
       <c r="I74" s="7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
@@ -4883,21 +5082,21 @@
         <v>18</v>
       </c>
       <c r="E75" s="7">
-        <v>7095749</v>
+        <v>7401165</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G75" s="7" t="str">
+        <v>74</v>
+      </c>
+      <c r="G75" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C75,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C75,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
         <v>Sun / 11a-3p</v>
       </c>
-      <c r="H75" s="7" t="str">
+      <c r="H75" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D75,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D75,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
         <v>Sun / 7p-11p</v>
       </c>
       <c r="I75" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -4914,21 +5113,21 @@
         <v>18</v>
       </c>
       <c r="E76" s="7">
-        <v>7091824</v>
+        <v>7401949</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G76" s="7" t="str">
+        <v>75</v>
+      </c>
+      <c r="G76" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C76,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C76,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
         <v>Sun / 11a-3p</v>
       </c>
-      <c r="H76" s="7" t="str">
+      <c r="H76" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D76,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D76,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
         <v>Sun / 7p-11p</v>
       </c>
       <c r="I76" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
@@ -4945,21 +5144,21 @@
         <v>18</v>
       </c>
       <c r="E77" s="7">
-        <v>7402915</v>
+        <v>7401950</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G77" s="7" t="str">
+        <v>76</v>
+      </c>
+      <c r="G77" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C77,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C77,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
         <v>Sun / 11a-3p</v>
       </c>
-      <c r="H77" s="7" t="str">
+      <c r="H77" s="2" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D77,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D77,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
         <v>Sun / 7p-11p</v>
       </c>
       <c r="I77" s="7" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
@@ -4976,10 +5175,10 @@
         <v>18</v>
       </c>
       <c r="E78" s="7">
-        <v>7051907</v>
+        <v>7095749</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G78" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C78,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C78,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -4990,7 +5189,7 @@
         <v>Sun / 7p-11p</v>
       </c>
       <c r="I78" s="7" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
@@ -5007,10 +5206,10 @@
         <v>18</v>
       </c>
       <c r="E79" s="7">
-        <v>7400976</v>
+        <v>7091824</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="G79" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C79,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C79,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -5021,7 +5220,7 @@
         <v>Sun / 7p-11p</v>
       </c>
       <c r="I79" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
@@ -5038,10 +5237,10 @@
         <v>18</v>
       </c>
       <c r="E80" s="7">
-        <v>7400954</v>
+        <v>7402915</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="G80" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C80,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C80,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -5052,7 +5251,7 @@
         <v>Sun / 7p-11p</v>
       </c>
       <c r="I80" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -5069,10 +5268,10 @@
         <v>18</v>
       </c>
       <c r="E81" s="7">
-        <v>7051890</v>
+        <v>7051907</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="G81" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C81,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C81,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -5083,7 +5282,7 @@
         <v>Sun / 7p-11p</v>
       </c>
       <c r="I81" s="7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
@@ -5100,10 +5299,10 @@
         <v>18</v>
       </c>
       <c r="E82" s="7">
-        <v>7051891</v>
+        <v>7400976</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="G82" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C82,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C82,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -5114,7 +5313,7 @@
         <v>Sun / 7p-11p</v>
       </c>
       <c r="I82" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
@@ -5130,11 +5329,11 @@
       <c r="D83" s="2">
         <v>18</v>
       </c>
-      <c r="E83" s="13">
-        <v>7403004</v>
+      <c r="E83" s="7">
+        <v>7400954</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="G83" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C83,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C83,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -5145,7 +5344,7 @@
         <v>Sun / 7p-11p</v>
       </c>
       <c r="I83" s="7" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
@@ -5162,10 +5361,10 @@
         <v>18</v>
       </c>
       <c r="E84" s="7">
-        <v>7095152</v>
+        <v>7051890</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G84" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C84,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C84,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -5176,7 +5375,7 @@
         <v>Sun / 7p-11p</v>
       </c>
       <c r="I84" s="7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
@@ -5193,10 +5392,10 @@
         <v>18</v>
       </c>
       <c r="E85" s="7">
-        <v>7095156</v>
+        <v>7051891</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="G85" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C85,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C85,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -5207,7 +5406,7 @@
         <v>Sun / 7p-11p</v>
       </c>
       <c r="I85" s="7" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
@@ -5223,11 +5422,11 @@
       <c r="D86" s="2">
         <v>18</v>
       </c>
-      <c r="E86" s="7">
-        <v>7051908</v>
+      <c r="E86" s="13">
+        <v>7403004</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="G86" s="7" t="str">
         <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C86,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C86,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
@@ -5238,7 +5437,131 @@
         <v>Sun / 7p-11p</v>
       </c>
       <c r="I86" s="7" t="s">
-        <v>204</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="2">
+        <v>1</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" s="2">
+        <v>16</v>
+      </c>
+      <c r="D87" s="2">
+        <v>18</v>
+      </c>
+      <c r="E87" s="7">
+        <v>7095152</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G87" s="7" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C87,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C87,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Sun / 11a-3p</v>
+      </c>
+      <c r="H87" s="7" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D87,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D87,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Sun / 7p-11p</v>
+      </c>
+      <c r="I87" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="2">
+        <v>1</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" s="2">
+        <v>16</v>
+      </c>
+      <c r="D88" s="2">
+        <v>18</v>
+      </c>
+      <c r="E88" s="7">
+        <v>7095156</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G88" s="7" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C88,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C88,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Sun / 11a-3p</v>
+      </c>
+      <c r="H88" s="7" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D88,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D88,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Sun / 7p-11p</v>
+      </c>
+      <c r="I88" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" s="2">
+        <v>1</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89" s="2">
+        <v>16</v>
+      </c>
+      <c r="D89" s="2">
+        <v>18</v>
+      </c>
+      <c r="E89" s="7">
+        <v>7051908</v>
+      </c>
+      <c r="F89" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G89" s="7" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C89,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C89,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Sun / 11a-3p</v>
+      </c>
+      <c r="H89" s="7" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D89,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D89,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Sun / 7p-11p</v>
+      </c>
+      <c r="I89" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="2">
+        <v>1</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" s="2">
+        <v>16</v>
+      </c>
+      <c r="D90" s="2">
+        <v>18</v>
+      </c>
+      <c r="E90" s="7">
+        <v>7104754</v>
+      </c>
+      <c r="F90" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G90" s="7" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!C90,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!C90,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Sun / 11a-3p</v>
+      </c>
+      <c r="H90" s="7" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(Assignment_List!D90,Slot_Legend!$A$2:$C$25,2,FALSE)," / ", VLOOKUP(Assignment_List!D90,Slot_Legend!$A$2:$C$25,3,FALSE))</f>
+        <v>Sun / 7p-11p</v>
+      </c>
+      <c r="I90" s="7" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -5550,10 +5873,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27494956-B098-494C-8CA2-BB2D03266D8E}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5602,7 +5925,7 @@
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>32</v>
@@ -5612,7 +5935,7 @@
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>32</v>
@@ -5692,7 +6015,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>37</v>
@@ -5722,7 +6045,7 @@
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>39</v>
@@ -5842,7 +6165,7 @@
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>50</v>
@@ -5872,7 +6195,7 @@
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>53</v>
@@ -5882,7 +6205,7 @@
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>54</v>
@@ -5892,7 +6215,7 @@
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>55</v>
@@ -5902,7 +6225,7 @@
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>56</v>
@@ -5942,17 +6265,17 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>59</v>
@@ -5972,7 +6295,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>61</v>
@@ -6002,7 +6325,7 @@
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>63</v>
@@ -6070,7 +6393,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B52" s="10" t="s">
         <v>68</v>
@@ -6086,7 +6409,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>70</v>
@@ -6094,7 +6417,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>71</v>
@@ -6102,7 +6425,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>72</v>
@@ -6110,7 +6433,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>72</v>
@@ -6118,7 +6441,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>72</v>
@@ -6126,7 +6449,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B59" s="10" t="s">
         <v>72</v>
@@ -6134,7 +6457,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B60" s="10" t="s">
         <v>72</v>
@@ -6142,10 +6465,66 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>